<commit_message>
Fix SQL pipeline v1: stable views, GLM baseline notebook, env setup
</commit_message>
<xml_diff>
--- a/data/raw/excel/VM_Spatial_Unit.xlsx
+++ b/data/raw/excel/VM_Spatial_Unit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c55ba288b6d60b4a/gvs-kyiv/data/raw/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{89FAC55D-6C0F-4A44-A7FA-2A5A0F8C5FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3FE806F-ED70-42C5-9D7E-4B34E57728D2}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{89FAC55D-6C0F-4A44-A7FA-2A5A0F8C5FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BA5E34E-F44C-46D5-BC39-1C361574D833}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="24500" windowHeight="19690" xr2:uid="{973263AB-F4B6-4F66-AB53-E1A53EFE3A77}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="23230" windowHeight="19690" xr2:uid="{973263AB-F4B6-4F66-AB53-E1A53EFE3A77}"/>
   </bookViews>
   <sheets>
     <sheet name="Spatial_Unit" sheetId="1" r:id="rId1"/>
@@ -3028,9 +3028,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AY155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL1" sqref="AL1"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI130" sqref="AI130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -3206,7 +3206,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:51" ht="79.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:51" ht="79.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4620,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:51" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:51" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -6292,7 +6292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -6668,7 +6668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -7690,7 +7690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -8074,7 +8074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -8330,7 +8330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -8586,7 +8586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -8714,7 +8714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -8844,7 +8844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -8968,7 +8968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -9098,7 +9098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -9226,7 +9226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -9358,7 +9358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -9488,7 +9488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -9618,7 +9618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -9740,7 +9740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -9868,7 +9868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -9996,7 +9996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -10252,7 +10252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -10382,7 +10382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -10516,7 +10516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -10646,7 +10646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -10776,7 +10776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -11426,7 +11426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -11556,7 +11556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -11688,7 +11688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -11822,7 +11822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -11956,7 +11956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:51" ht="65" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:51" ht="65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -12086,7 +12086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -12216,7 +12216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -12348,7 +12348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -12478,7 +12478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -12608,7 +12608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -12734,7 +12734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -12866,7 +12866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -12996,7 +12996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -13126,7 +13126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -13256,7 +13256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -13386,7 +13386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -13516,7 +13516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -13646,7 +13646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -13906,7 +13906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -14036,7 +14036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -14166,7 +14166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -14296,7 +14296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -14426,7 +14426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -14558,7 +14558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -14690,7 +14690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -14822,7 +14822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -14952,7 +14952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -15086,7 +15086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -15218,7 +15218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -15490,7 +15490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -15754,7 +15754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -15886,7 +15886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -16018,7 +16018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -16150,7 +16150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -16282,7 +16282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -16414,7 +16414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -16550,7 +16550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -16682,7 +16682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -16816,7 +16816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -16950,7 +16950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -17084,7 +17084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -17216,7 +17216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -17348,7 +17348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -17480,7 +17480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -17614,7 +17614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -17748,7 +17748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -17882,7 +17882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -18014,7 +18014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -18146,7 +18146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -18278,7 +18278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -18410,7 +18410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -18546,7 +18546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -18680,7 +18680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -18814,7 +18814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -18948,7 +18948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -19082,7 +19082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -19218,7 +19218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -19352,7 +19352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -19486,7 +19486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -19622,7 +19622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -19758,7 +19758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -20030,7 +20030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:51" ht="26" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:51" ht="26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -20168,7 +20168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -20304,7 +20304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -20438,7 +20438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:51" ht="91" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:51" ht="91" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -20572,7 +20572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -20704,7 +20704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -20834,7 +20834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -21098,7 +21098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -21228,7 +21228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -21360,7 +21360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -21490,7 +21490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -21620,7 +21620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -21752,7 +21752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -21882,7 +21882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -22012,7 +22012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -22142,7 +22142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -22272,7 +22272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -22402,7 +22402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -22666,7 +22666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -22796,7 +22796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -22930,7 +22930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -23062,7 +23062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -23194,7 +23194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:51" ht="78" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:51" ht="78" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -23326,6 +23326,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AX155" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="8000000000:75:792:0102"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="37">
       <filters>
         <filter val="5"/>

</xml_diff>